<commit_message>
bf: add bf forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Burkina Faso/nov 2023/bf_202311_sch_impact_assessment_1_sites.xlsx
+++ b/SCH-STH/Impact assessments/Burkina Faso/nov 2023/bf_202311_sch_impact_assessment_1_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Burkina Faso\nov 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5531C0A7-B18D-4C93-919A-94A06310B972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32203E23-FC0C-479B-8AFC-3C0F58B18DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="283">
   <si>
     <t>type</t>
   </si>
@@ -660,24 +660,12 @@
     <t>Zorgho</t>
   </si>
   <si>
-    <t>Boudry</t>
-  </si>
-  <si>
-    <t>Zam</t>
-  </si>
-  <si>
     <t>Meguet</t>
   </si>
   <si>
     <t>Mogtedo</t>
   </si>
   <si>
-    <t>Salogo</t>
-  </si>
-  <si>
-    <t>Zoungou</t>
-  </si>
-  <si>
     <t>Boussé</t>
   </si>
   <si>
@@ -843,12 +831,6 @@
     <t>Ziglakoulpélé</t>
   </si>
   <si>
-    <t>(BF - NIvembre 2023) impact schisto - 1. Formulaire Village V2</t>
-  </si>
-  <si>
-    <t>bf_202311_sch_impact_assessment_1_sites_v2</t>
-  </si>
-  <si>
     <t>Absouya</t>
   </si>
   <si>
@@ -877,6 +859,33 @@
   </si>
   <si>
     <t>Bagre</t>
+  </si>
+  <si>
+    <t>bf_202311_sch_impact_assessment_1_sites_v2_1</t>
+  </si>
+  <si>
+    <t>Bourma</t>
+  </si>
+  <si>
+    <t>Sankuissi</t>
+  </si>
+  <si>
+    <t>Dawaka</t>
+  </si>
+  <si>
+    <t>Talembika</t>
+  </si>
+  <si>
+    <t>Koumséogo</t>
+  </si>
+  <si>
+    <t>Wada</t>
+  </si>
+  <si>
+    <t>Rapadama Ud</t>
+  </si>
+  <si>
+    <t>(BF - Novembre 2023) impact schisto - 1. Formulaire Village V2.1</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1000,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2273,13 +2282,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A64" sqref="A64:XFD130"/>
+      <selection pane="bottomRight" activeCell="A64" sqref="A64:XFD133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
@@ -2930,10 +2939,10 @@
         <v>95</v>
       </c>
       <c r="B64" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C64" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2959,13 +2968,13 @@
         <v>96</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D67" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2973,13 +2982,13 @@
         <v>96</v>
       </c>
       <c r="B68" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C68" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D68" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2987,13 +2996,13 @@
         <v>96</v>
       </c>
       <c r="B69" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C69" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3001,10 +3010,10 @@
         <v>96</v>
       </c>
       <c r="B70" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C70" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>205</v>
@@ -3015,10 +3024,10 @@
         <v>96</v>
       </c>
       <c r="B71" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C71" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>205</v>
@@ -3046,13 +3055,13 @@
         <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E74" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
@@ -3062,13 +3071,13 @@
         <v>97</v>
       </c>
       <c r="B75" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C75" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E75" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
@@ -3078,13 +3087,13 @@
         <v>97</v>
       </c>
       <c r="B76" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C76" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E76" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
@@ -3094,13 +3103,13 @@
         <v>97</v>
       </c>
       <c r="B77" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C77" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E77" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
@@ -3110,13 +3119,13 @@
         <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C78" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E78" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
@@ -3126,13 +3135,13 @@
         <v>97</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C79" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E79" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
@@ -3142,13 +3151,13 @@
         <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C80" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E80" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
@@ -3158,13 +3167,13 @@
         <v>97</v>
       </c>
       <c r="B81" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C81" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E81" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
@@ -3174,13 +3183,13 @@
         <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C82" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E82" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
@@ -3190,13 +3199,13 @@
         <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C83" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E83" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
@@ -3206,13 +3215,13 @@
         <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E84" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
@@ -3222,13 +3231,13 @@
         <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C85" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E85" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
@@ -3238,13 +3247,13 @@
         <v>97</v>
       </c>
       <c r="B86" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C86" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E86" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
@@ -3254,13 +3263,13 @@
         <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C87" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E87" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
@@ -3270,13 +3279,13 @@
         <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C88" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E88" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -3286,13 +3295,13 @@
         <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C89" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E89" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -3302,13 +3311,13 @@
         <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C90" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E90" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -3318,13 +3327,13 @@
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C91" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E91" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
@@ -3334,13 +3343,13 @@
         <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C92" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E92" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -3350,13 +3359,13 @@
         <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C93" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E93" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
@@ -3366,13 +3375,13 @@
         <v>97</v>
       </c>
       <c r="B94" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C94" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E94" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
@@ -3382,13 +3391,13 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C95" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E95" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
@@ -3398,13 +3407,13 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C96" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E96" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
@@ -3414,13 +3423,13 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C97" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E97" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
@@ -3430,13 +3439,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C98" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E98" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
@@ -3446,13 +3455,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C99" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E99" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
@@ -3462,13 +3471,13 @@
         <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C100" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E100" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
@@ -3478,13 +3487,13 @@
         <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C101" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E101" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
@@ -3494,13 +3503,13 @@
         <v>97</v>
       </c>
       <c r="B102" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C102" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E102" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
@@ -3510,13 +3519,13 @@
         <v>97</v>
       </c>
       <c r="B103" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C103" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E103" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
@@ -3526,13 +3535,13 @@
         <v>97</v>
       </c>
       <c r="B104" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C104" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E104" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
@@ -3542,13 +3551,13 @@
         <v>97</v>
       </c>
       <c r="B105" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C105" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E105" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
@@ -3558,13 +3567,13 @@
         <v>97</v>
       </c>
       <c r="B106" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C106" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E106" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
@@ -3574,13 +3583,13 @@
         <v>97</v>
       </c>
       <c r="B107" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C107" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E107" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
@@ -3590,13 +3599,13 @@
         <v>97</v>
       </c>
       <c r="B108" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C108" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E108" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
@@ -3606,13 +3615,13 @@
         <v>97</v>
       </c>
       <c r="B109" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C109" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E109" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F109" s="6"/>
       <c r="G109" s="6"/>
@@ -3622,13 +3631,13 @@
         <v>97</v>
       </c>
       <c r="B110" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C110" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E110" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
@@ -3638,13 +3647,13 @@
         <v>97</v>
       </c>
       <c r="B111" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C111" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E111" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F111" s="6"/>
       <c r="G111" s="6"/>
@@ -3654,13 +3663,13 @@
         <v>97</v>
       </c>
       <c r="B112" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C112" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E112" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F112" s="6"/>
       <c r="G112" s="6"/>
@@ -3670,13 +3679,13 @@
         <v>97</v>
       </c>
       <c r="B113" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C113" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E113" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
@@ -3686,13 +3695,13 @@
         <v>97</v>
       </c>
       <c r="B114" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C114" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E114" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
@@ -3702,13 +3711,13 @@
         <v>97</v>
       </c>
       <c r="B115" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C115" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E115" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F115" s="6"/>
       <c r="G115" s="6"/>
@@ -3718,13 +3727,13 @@
         <v>97</v>
       </c>
       <c r="B116" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C116" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E116" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
@@ -3734,13 +3743,13 @@
         <v>97</v>
       </c>
       <c r="B117" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C117" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E117" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F117" s="6"/>
       <c r="G117" s="6"/>
@@ -3750,13 +3759,13 @@
         <v>97</v>
       </c>
       <c r="B118" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C118" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E118" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
@@ -3766,13 +3775,13 @@
         <v>97</v>
       </c>
       <c r="B119" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C119" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E119" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
@@ -3782,13 +3791,13 @@
         <v>97</v>
       </c>
       <c r="B120" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C120" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E120" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
@@ -3798,13 +3807,13 @@
         <v>97</v>
       </c>
       <c r="B121" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C121" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E121" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
@@ -3814,13 +3823,13 @@
         <v>97</v>
       </c>
       <c r="B122" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C122" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E122" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
@@ -3830,13 +3839,13 @@
         <v>97</v>
       </c>
       <c r="B123" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C123" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E123" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F123" s="6"/>
       <c r="G123" s="6"/>
@@ -3846,10 +3855,10 @@
         <v>97</v>
       </c>
       <c r="B124" t="s">
-        <v>207</v>
+        <v>275</v>
       </c>
       <c r="C124" t="s">
-        <v>207</v>
+        <v>275</v>
       </c>
       <c r="E124" t="s">
         <v>206</v>
@@ -3862,10 +3871,10 @@
         <v>97</v>
       </c>
       <c r="B125" t="s">
-        <v>209</v>
+        <v>277</v>
       </c>
       <c r="C125" t="s">
-        <v>209</v>
+        <v>277</v>
       </c>
       <c r="E125" t="s">
         <v>206</v>
@@ -3878,10 +3887,10 @@
         <v>97</v>
       </c>
       <c r="B126" t="s">
-        <v>210</v>
+        <v>279</v>
       </c>
       <c r="C126" t="s">
-        <v>210</v>
+        <v>279</v>
       </c>
       <c r="E126" t="s">
         <v>206</v>
@@ -3894,10 +3903,10 @@
         <v>97</v>
       </c>
       <c r="B127" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C127" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E127" t="s">
         <v>206</v>
@@ -3926,10 +3935,10 @@
         <v>97</v>
       </c>
       <c r="B129" t="s">
-        <v>206</v>
+        <v>281</v>
       </c>
       <c r="C129" t="s">
-        <v>206</v>
+        <v>281</v>
       </c>
       <c r="E129" t="s">
         <v>206</v>
@@ -3942,16 +3951,58 @@
         <v>97</v>
       </c>
       <c r="B130" t="s">
-        <v>212</v>
+        <v>276</v>
       </c>
       <c r="C130" t="s">
-        <v>212</v>
+        <v>276</v>
       </c>
       <c r="E130" t="s">
         <v>206</v>
       </c>
       <c r="F130" s="6"/>
       <c r="G130" s="6"/>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>97</v>
+      </c>
+      <c r="B131" t="s">
+        <v>278</v>
+      </c>
+      <c r="C131" t="s">
+        <v>278</v>
+      </c>
+      <c r="E131" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>97</v>
+      </c>
+      <c r="B132" t="s">
+        <v>280</v>
+      </c>
+      <c r="C132" t="s">
+        <v>280</v>
+      </c>
+      <c r="E132" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
+        <v>97</v>
+      </c>
+      <c r="B133" t="s">
+        <v>206</v>
+      </c>
+      <c r="C133" t="s">
+        <v>206</v>
+      </c>
+      <c r="E133" t="s">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -4026,12 +4077,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="52.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.25" style="18" customWidth="1"/>
     <col min="3" max="16384" width="10.5" style="18"/>
   </cols>
@@ -4052,10 +4103,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="17" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>16</v>
@@ -4074,8 +4125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB163701-A23A-4287-9ABE-ADE1596168A2}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4084,6 +4135,7 @@
     <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.75" bestFit="1" customWidth="1"/>
@@ -4130,23 +4182,23 @@
       <c r="C2" t="s">
         <v>206</v>
       </c>
-      <c r="D2" t="s">
-        <v>207</v>
+      <c r="D2" s="20" t="s">
+        <v>275</v>
       </c>
       <c r="G2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="I2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="L2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -4159,23 +4211,23 @@
       <c r="C3" t="s">
         <v>206</v>
       </c>
-      <c r="D3" t="s">
-        <v>207</v>
+      <c r="D3" s="20" t="s">
+        <v>276</v>
       </c>
       <c r="G3" t="s">
         <v>205</v>
       </c>
       <c r="I3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="L3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -4188,20 +4240,20 @@
       <c r="C4" t="s">
         <v>206</v>
       </c>
-      <c r="D4" t="s">
-        <v>208</v>
+      <c r="D4" s="20" t="s">
+        <v>277</v>
       </c>
       <c r="I4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M4" t="s">
         <v>213</v>
-      </c>
-      <c r="M4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -4214,20 +4266,20 @@
       <c r="C5" t="s">
         <v>206</v>
       </c>
-      <c r="D5" t="s">
-        <v>209</v>
+      <c r="D5" s="20" t="s">
+        <v>207</v>
       </c>
       <c r="I5" t="s">
         <v>205</v>
       </c>
       <c r="J5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="L5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -4240,20 +4292,20 @@
       <c r="C6" t="s">
         <v>206</v>
       </c>
-      <c r="D6" t="s">
-        <v>210</v>
+      <c r="D6" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="I6" t="s">
         <v>205</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="L6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -4266,8 +4318,8 @@
       <c r="C7" t="s">
         <v>206</v>
       </c>
-      <c r="D7" t="s">
-        <v>210</v>
+      <c r="D7" s="20" t="s">
+        <v>281</v>
       </c>
       <c r="I7" t="s">
         <v>205</v>
@@ -4276,10 +4328,10 @@
         <v>206</v>
       </c>
       <c r="L7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -4292,14 +4344,14 @@
       <c r="C8" t="s">
         <v>206</v>
       </c>
-      <c r="D8" t="s">
-        <v>208</v>
+      <c r="D8" s="20" t="s">
+        <v>278</v>
       </c>
       <c r="L8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -4312,14 +4364,14 @@
       <c r="C9" t="s">
         <v>206</v>
       </c>
-      <c r="D9" t="s">
-        <v>211</v>
+      <c r="D9" s="20" t="s">
+        <v>279</v>
       </c>
       <c r="L9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -4332,14 +4384,14 @@
       <c r="C10" t="s">
         <v>206</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="20" t="s">
         <v>206</v>
       </c>
       <c r="L10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M10" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -4352,14 +4404,14 @@
       <c r="C11" t="s">
         <v>206</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="L11" t="s">
+        <v>209</v>
+      </c>
+      <c r="M11" t="s">
         <v>212</v>
-      </c>
-      <c r="L11" t="s">
-        <v>213</v>
-      </c>
-      <c r="M11" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -4367,19 +4419,19 @@
         <v>205</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D12" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="L12" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M12" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -4387,19 +4439,19 @@
         <v>205</v>
       </c>
       <c r="B13" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D13" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="L13" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -4407,19 +4459,19 @@
         <v>205</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D14" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L14" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M14" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -4427,19 +4479,19 @@
         <v>205</v>
       </c>
       <c r="B15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C15" t="s">
         <v>213</v>
       </c>
-      <c r="C15" t="s">
-        <v>217</v>
-      </c>
       <c r="D15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="L15" t="s">
+        <v>232</v>
+      </c>
+      <c r="M15" t="s">
         <v>236</v>
-      </c>
-      <c r="M15" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -4447,19 +4499,19 @@
         <v>205</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="L16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M16" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -4467,19 +4519,19 @@
         <v>205</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D17" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="L17" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M17" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -4487,19 +4539,19 @@
         <v>205</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D18" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="L18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M18" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -4507,19 +4559,19 @@
         <v>205</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D19" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="L19" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M19" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -4527,19 +4579,19 @@
         <v>205</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C20" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D20" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="L20" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M20" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -4547,19 +4599,19 @@
         <v>205</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="L21" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M21" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -4567,19 +4619,19 @@
         <v>205</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C22" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D22" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="L22" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -4587,19 +4639,19 @@
         <v>205</v>
       </c>
       <c r="B23" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C23" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D23" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L23" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M23" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -4607,19 +4659,19 @@
         <v>205</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C24" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D24" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L24" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M24" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -4627,19 +4679,19 @@
         <v>205</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C25" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D25" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L25" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M25" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -4647,19 +4699,19 @@
         <v>205</v>
       </c>
       <c r="B26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C26" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D26" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="L26" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M26" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -4667,19 +4719,19 @@
         <v>205</v>
       </c>
       <c r="B27" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C27" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D27" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="L27" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M27" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -4687,19 +4739,19 @@
         <v>205</v>
       </c>
       <c r="B28" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" t="s">
+        <v>221</v>
+      </c>
+      <c r="D28" t="s">
         <v>225</v>
       </c>
-      <c r="C28" t="s">
-        <v>225</v>
-      </c>
-      <c r="D28" t="s">
-        <v>229</v>
-      </c>
       <c r="L28" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M28" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -4707,19 +4759,19 @@
         <v>205</v>
       </c>
       <c r="B29" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C29" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D29" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="L29" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M29" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -4727,19 +4779,19 @@
         <v>205</v>
       </c>
       <c r="B30" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C30" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D30" t="s">
+        <v>227</v>
+      </c>
+      <c r="L30" t="s">
         <v>231</v>
       </c>
-      <c r="L30" t="s">
-        <v>235</v>
-      </c>
       <c r="M30" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -4747,601 +4799,619 @@
         <v>205</v>
       </c>
       <c r="B31" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C31" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D31" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="L31" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M31" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B32" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C32" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D32" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="L32" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M32" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B33" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C33" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D33" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L33" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M33" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C34" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D34" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="L34" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M34" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B35" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C35" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="L35" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M35" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B36" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C36" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D36" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="L36" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M36" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B37" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C37" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D37" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="L37" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M37" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B38" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C38" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D38" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="L38" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M38" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B39" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D39" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="L39" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M39" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B40" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C40" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D40" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="L40" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M40" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B41" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C41" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="L41" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B42" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C42" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D42" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="L42" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M42" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B43" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C43" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D43" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="L43" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M43" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B44" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D44" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L44" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M44" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B45" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C45" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D45" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="L45" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M45" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B46" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C46" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D46" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="L46" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M46" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B47" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C47" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D47" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="L47" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M47" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B48" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C48" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D48" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="L48" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M48" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B49" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C49" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D49" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="L49" t="s">
+        <v>221</v>
+      </c>
+      <c r="M49" t="s">
         <v>225</v>
-      </c>
-      <c r="M49" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B50" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C50" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D50" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="L50" s="20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M50" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B51" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C51" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D51" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="L51" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M51" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" t="s">
+        <v>229</v>
+      </c>
+      <c r="B52" t="s">
+        <v>232</v>
+      </c>
+      <c r="C52" t="s">
         <v>233</v>
       </c>
-      <c r="B52" t="s">
-        <v>236</v>
-      </c>
-      <c r="C52" t="s">
-        <v>237</v>
-      </c>
       <c r="D52" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="L52" t="s">
         <v>206</v>
       </c>
-      <c r="M52" t="s">
-        <v>207</v>
+      <c r="M52" s="20" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" t="s">
+        <v>229</v>
+      </c>
+      <c r="B53" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" t="s">
         <v>233</v>
       </c>
-      <c r="B53" t="s">
-        <v>236</v>
-      </c>
-      <c r="C53" t="s">
-        <v>237</v>
-      </c>
       <c r="D53" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="L53" t="s">
         <v>206</v>
       </c>
-      <c r="M53" t="s">
-        <v>209</v>
+      <c r="M53" s="20" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B54" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C54" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D54" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="L54" t="s">
         <v>206</v>
       </c>
-      <c r="M54" t="s">
-        <v>210</v>
+      <c r="M54" s="20" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B55" t="s">
+        <v>232</v>
+      </c>
+      <c r="C55" t="s">
+        <v>232</v>
+      </c>
+      <c r="D55" t="s">
         <v>236</v>
-      </c>
-      <c r="C55" t="s">
-        <v>236</v>
-      </c>
-      <c r="D55" t="s">
-        <v>240</v>
       </c>
       <c r="L55" t="s">
         <v>206</v>
       </c>
-      <c r="M55" t="s">
-        <v>211</v>
+      <c r="M55" s="20" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" t="s">
+        <v>229</v>
+      </c>
+      <c r="B56" t="s">
+        <v>232</v>
+      </c>
+      <c r="C56" t="s">
         <v>233</v>
       </c>
-      <c r="B56" t="s">
-        <v>236</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>237</v>
-      </c>
-      <c r="D56" t="s">
-        <v>241</v>
       </c>
       <c r="L56" t="s">
         <v>206</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M56" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B57" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C57" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D57" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="L57" t="s">
         <v>206</v>
       </c>
-      <c r="M57" t="s">
-        <v>206</v>
+      <c r="M57" s="20" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B58" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C58" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D58" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="L58" t="s">
         <v>206</v>
       </c>
-      <c r="M58" t="s">
-        <v>212</v>
+      <c r="M58" s="20" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B59" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C59" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D59" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="L59" t="s">
+        <v>206</v>
+      </c>
+      <c r="M59" s="20" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B60" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C60" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D60" t="s">
-        <v>245</v>
+        <v>241</v>
+      </c>
+      <c r="L60" t="s">
+        <v>206</v>
+      </c>
+      <c r="M60" s="20" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B61" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C61" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D61" t="s">
-        <v>267</v>
+        <v>263</v>
+      </c>
+      <c r="L61" t="s">
+        <v>206</v>
+      </c>
+      <c r="M61" s="20" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>